<commit_message>
Update status of pm10,pm25
</commit_message>
<xml_diff>
--- a/서울시_미세먼지데이터.xlsx
+++ b/서울시_미세먼지데이터.xlsx
@@ -395,7 +395,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -415,29 +415,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.025</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.019</t>
+          <t>0.024</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>18</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>42</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -447,39 +447,39 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.003</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.062</t>
+          <t>0.026</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.023</t>
+          <t>0.030</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>48</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>64</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -489,39 +489,39 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.003</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.064</t>
+          <t>0.023</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.016</t>
+          <t>0.023</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>24</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>40</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -536,34 +536,34 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.6</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.070</t>
+          <t>0.026</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0.023</t>
+          <t>0.025</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>83</t>
+          <t>51</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -583,29 +583,29 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.076</t>
+          <t>0.028</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>0.024</t>
+          <t>0.023</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>47</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -625,29 +625,29 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.071</t>
+          <t>0.026</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.010</t>
+          <t>0.017</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>21</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>43</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -662,34 +662,34 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.095</t>
+          <t>0.041</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0.014</t>
+          <t>0.018</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>17</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>59</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -699,39 +699,39 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.002</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.4</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.085</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.012</t>
+          <t>0.021</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>20</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>48</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -746,34 +746,34 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.3</t>
+          <t>0.4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.063</t>
+          <t>0.025</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>0.053</t>
+          <t>0.034</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>25</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>88</t>
+          <t>56</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2020-05-30 13:00</t>
+          <t>2020-06-02 01:00</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -788,27 +788,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.4</t>
+          <t>0.5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.073</t>
+          <t>0.025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>0.015</t>
+          <t>0.027</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>22</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>86</t>
+          <t>45</t>
         </is>
       </c>
     </row>

</xml_diff>